<commit_message>
check XTT pivot templates
</commit_message>
<xml_diff>
--- a/src/zr_py000_report.xlsx.w3mi.data.xlsx
+++ b/src/zr_py000_report.xlsx.w3mi.data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{F923C966-709C-4E16-AC7B-0DA72F9339A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
     <sheet name="RawPivot" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="55" r:id="rId4"/>
+    <pivotCache cacheId="21" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -179,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -841,6 +842,60 @@
           <a:effectLst/>
         </c:spPr>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="30"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="33"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -855,7 +910,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Personnel Subarea - Sum of SUM_1</c:v>
+                  <c:v>{R-T-BTRTL} - Sum of SUM_1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -884,7 +939,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Personnel Area</c:v>
+                  <c:v>{R-T-WERKS}</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -916,7 +971,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Personnel Subarea - Sum of SUM_2</c:v>
+                  <c:v>{R-T-BTRTL} - Sum of SUM_2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -945,7 +1000,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Personnel Area</c:v>
+                  <c:v>{R-T-WERKS}</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1631,7 +1686,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1650,7 +1711,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="43964.487031018522" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44779.765166435187" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF37000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="TB_PIVOT"/>
   </cacheSource>
@@ -1672,7 +1733,7 @@
     </cacheField>
     <cacheField name="Personnel Subarea" numFmtId="0">
       <sharedItems count="1">
-        <s v="{R-T-BTRTL;type=integer}"/>
+        <s v="{R-T-BTRTL}"/>
       </sharedItems>
     </cacheField>
     <cacheField name="SUM_1" numFmtId="4">
@@ -1694,7 +1755,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="55" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable5" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A4:C8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisPage" subtotalTop="0" showAll="0">
@@ -1711,13 +1772,13 @@
     </pivotField>
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
       <items count="2">
-        <item n="Personnel Area" x="0"/>
+        <item n="{R-T-WERKS}" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="2">
-        <item n="Personnel Subarea" x="0"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1758,7 +1819,7 @@
     <dataField name="Sum of SUM_2" fld="5" baseField="2" baseItem="0" numFmtId="4"/>
   </dataFields>
   <chartFormats count="4">
-    <chartFormat chart="0" format="26" series="1">
+    <chartFormat chart="0" format="30" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1770,7 +1831,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="27">
+    <chartFormat chart="0" format="31">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1785,7 +1846,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="28" series="1">
+    <chartFormat chart="0" format="32" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1797,7 +1858,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="29">
+    <chartFormat chart="0" format="33">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1818,21 +1879,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TB_PIVOT" displayName="TB_PIVOT" ref="B2:H4" totalsRowCount="1">
-  <autoFilter ref="B2:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TB_PIVOT" displayName="TB_PIVOT" ref="B2:H4" totalsRowCount="1">
+  <autoFilter ref="B2:H3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Personnel Number" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Formatted Name of Employee"/>
-    <tableColumn id="3" name="Personnel Area"/>
-    <tableColumn id="4" name="Personnel Subarea"/>
-    <tableColumn id="5" name="SUM_1" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="SUM_2" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="7" name="SUM_3" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Personnel Number" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Formatted Name of Employee"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Personnel Area"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Personnel Subarea"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SUM_1" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="SUM_2" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="SUM_3" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2100,7 +2164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2205,17 +2269,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
@@ -2243,7 +2307,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2259,7 +2323,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B7" s="18">
         <v>0</v>
@@ -2286,7 +2350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>